<commit_message>
minor changes in template percents
</commit_message>
<xml_diff>
--- a/Projects/CCRUFIFA2018/Data/FIFA KPIs.xlsx
+++ b/Projects/CCRUFIFA2018/Data/FIFA KPIs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Permanent Concession" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,6 +41,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Permanent Concession'!$A$1:$AE$24</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Permanent Concession'!$A$1:$AE$24</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Permanent Concession'!$A$1:$AE$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Permanent Concession'!$A$1:$AE$24</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0" vbProcedure="false">FFF!$A$1:$AE$21</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0_0" vbProcedure="false">FFF!$A$1:$AE$21</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0_0_0" vbProcedure="false">FFF!$A$1:$AE$21</definedName>
@@ -63,6 +64,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">FFF!$A$1:$AE$21</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">FFF!$A$1:$AE$21</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">FFF!$A$1:$AE$21</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">FFF!$A$1:$AE$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -617,7 +619,7 @@
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="0%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -674,12 +676,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -809,7 +805,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -878,8 +874,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -906,6 +902,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1058,6 +1058,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1106,10 +1110,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1132,6 +1132,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1298,7 +1302,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1393,21 +1397,21 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.7449392712551"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.57085020242915"/>
@@ -1415,10 +1419,10 @@
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="24" min="22" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="28" min="26" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1619,7 +1623,7 @@
         <v>42</v>
       </c>
       <c r="V3" s="17" t="n">
-        <v>0.0286</v>
+        <v>0.0285715</v>
       </c>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -1684,7 +1688,7 @@
         <v>42</v>
       </c>
       <c r="V4" s="17" t="n">
-        <v>0.0286</v>
+        <v>0.0285715</v>
       </c>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
@@ -1749,7 +1753,7 @@
         <v>42</v>
       </c>
       <c r="V5" s="17" t="n">
-        <v>0.0286</v>
+        <v>0.028571</v>
       </c>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
@@ -1814,7 +1818,7 @@
         <v>42</v>
       </c>
       <c r="V6" s="17" t="n">
-        <v>0.0286</v>
+        <v>0.0285715</v>
       </c>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
@@ -1879,7 +1883,7 @@
         <v>42</v>
       </c>
       <c r="V7" s="17" t="n">
-        <v>0.0286</v>
+        <v>0.0285715</v>
       </c>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
@@ -1944,7 +1948,7 @@
         <v>42</v>
       </c>
       <c r="V8" s="17" t="n">
-        <v>0.0286</v>
+        <v>0.0285715</v>
       </c>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
@@ -2009,7 +2013,7 @@
         <v>42</v>
       </c>
       <c r="V9" s="17" t="n">
-        <v>0.0286</v>
+        <v>0.0285715</v>
       </c>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -2073,7 +2077,7 @@
       <c r="U10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="V10" s="17" t="n">
+      <c r="V10" s="24" t="n">
         <v>0.2</v>
       </c>
       <c r="W10" s="3"/>
@@ -2089,65 +2093,65 @@
       <c r="AE10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="34" t="s">
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34" t="s">
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="U11" s="29"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="34"/>
-      <c r="X11" s="34"/>
-      <c r="Y11" s="36" t="s">
+      <c r="U11" s="30"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="35"/>
+      <c r="X11" s="35"/>
+      <c r="Y11" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Z11" s="34"/>
-      <c r="AA11" s="34"/>
-      <c r="AB11" s="37"/>
-      <c r="AC11" s="38" t="s">
+      <c r="Z11" s="35"/>
+      <c r="AA11" s="35"/>
+      <c r="AB11" s="38"/>
+      <c r="AC11" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="AD11" s="37"/>
-      <c r="AE11" s="39"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="n">
+      <c r="A12" s="41" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="42" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -2175,12 +2179,12 @@
       <c r="U12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V12" s="42" t="n">
+      <c r="V12" s="43" t="n">
         <v>0.3</v>
       </c>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
-      <c r="Y12" s="36" t="s">
+      <c r="Y12" s="37" t="s">
         <v>71</v>
       </c>
       <c r="Z12" s="3"/>
@@ -2195,16 +2199,16 @@
       <c r="AE12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="n">
+      <c r="A13" s="41" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="44" t="s">
         <v>74</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -2215,10 +2219,10 @@
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="44" t="s">
+      <c r="I13" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="45" t="n">
+      <c r="J13" s="46" t="n">
         <v>54491472</v>
       </c>
       <c r="K13" s="16"/>
@@ -2244,7 +2248,7 @@
       <c r="U13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V13" s="46" t="n">
+      <c r="V13" s="47" t="n">
         <v>0.06</v>
       </c>
       <c r="W13" s="3"/>
@@ -2256,22 +2260,22 @@
         <v>3</v>
       </c>
       <c r="AC13" s="6"/>
-      <c r="AD13" s="41" t="s">
+      <c r="AD13" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="n">
+      <c r="A14" s="41" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="44" t="s">
         <v>76</v>
       </c>
       <c r="E14" s="11" t="s">
@@ -2282,10 +2286,10 @@
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="44" t="s">
+      <c r="I14" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="48" t="s">
         <v>77</v>
       </c>
       <c r="K14" s="16"/>
@@ -2311,7 +2315,7 @@
       <c r="U14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V14" s="46" t="n">
+      <c r="V14" s="47" t="n">
         <v>0.06</v>
       </c>
       <c r="W14" s="3"/>
@@ -2323,22 +2327,22 @@
         <v>3</v>
       </c>
       <c r="AC14" s="6"/>
-      <c r="AD14" s="41" t="s">
+      <c r="AD14" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="40" t="n">
+      <c r="A15" s="41" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="44" t="s">
         <v>79</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -2349,10 +2353,10 @@
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="44" t="s">
+      <c r="I15" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="45" t="n">
+      <c r="J15" s="46" t="n">
         <v>5449000131836</v>
       </c>
       <c r="K15" s="16"/>
@@ -2378,7 +2382,7 @@
       <c r="U15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V15" s="46" t="n">
+      <c r="V15" s="47" t="n">
         <v>0.02667</v>
       </c>
       <c r="W15" s="3"/>
@@ -2390,22 +2394,22 @@
         <v>3</v>
       </c>
       <c r="AC15" s="6"/>
-      <c r="AD15" s="41" t="s">
+      <c r="AD15" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="n">
+      <c r="A16" s="41" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="44" t="s">
         <v>81</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -2416,10 +2420,10 @@
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="44" t="s">
+      <c r="I16" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="45" t="n">
+      <c r="J16" s="46" t="n">
         <v>40822938</v>
       </c>
       <c r="K16" s="16"/>
@@ -2445,7 +2449,7 @@
       <c r="U16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V16" s="46" t="n">
+      <c r="V16" s="47" t="n">
         <v>0.01332</v>
       </c>
       <c r="W16" s="3"/>
@@ -2457,22 +2461,22 @@
         <v>3</v>
       </c>
       <c r="AC16" s="6"/>
-      <c r="AD16" s="41" t="s">
+      <c r="AD16" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="n">
+      <c r="A17" s="41" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="44" t="s">
         <v>83</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -2483,10 +2487,10 @@
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
-      <c r="I17" s="44" t="s">
+      <c r="I17" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="45" t="n">
+      <c r="J17" s="46" t="n">
         <v>54491069</v>
       </c>
       <c r="K17" s="16"/>
@@ -2512,7 +2516,7 @@
       <c r="U17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V17" s="46" t="n">
+      <c r="V17" s="47" t="n">
         <v>0.02001</v>
       </c>
       <c r="W17" s="3"/>
@@ -2524,22 +2528,22 @@
         <v>3</v>
       </c>
       <c r="AC17" s="6"/>
-      <c r="AD17" s="41" t="s">
+      <c r="AD17" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="40" t="n">
+      <c r="A18" s="41" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="49" t="s">
         <v>85</v>
       </c>
       <c r="E18" s="11" t="s">
@@ -2579,7 +2583,7 @@
       <c r="U18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V18" s="46" t="n">
+      <c r="V18" s="47" t="n">
         <v>0.02</v>
       </c>
       <c r="W18" s="3"/>
@@ -2591,22 +2595,22 @@
         <v>3</v>
       </c>
       <c r="AC18" s="6"/>
-      <c r="AD18" s="41" t="s">
+      <c r="AD18" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="40" t="n">
+      <c r="A19" s="41" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="49" t="s">
         <v>87</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -2646,7 +2650,7 @@
       <c r="U19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V19" s="46" t="n">
+      <c r="V19" s="47" t="n">
         <v>0.06</v>
       </c>
       <c r="W19" s="3"/>
@@ -2658,22 +2662,22 @@
         <v>3</v>
       </c>
       <c r="AC19" s="6"/>
-      <c r="AD19" s="41" t="s">
+      <c r="AD19" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="40" t="n">
+      <c r="A20" s="41" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="44" t="s">
         <v>89</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -2684,10 +2688,10 @@
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="45" t="n">
+      <c r="J20" s="46" t="n">
         <v>5449000189301</v>
       </c>
       <c r="K20" s="16"/>
@@ -2713,7 +2717,7 @@
       <c r="U20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V20" s="46" t="n">
+      <c r="V20" s="47" t="n">
         <v>0.02</v>
       </c>
       <c r="W20" s="3"/>
@@ -2725,22 +2729,22 @@
         <v>3</v>
       </c>
       <c r="AC20" s="6"/>
-      <c r="AD20" s="41" t="s">
+      <c r="AD20" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="40" t="n">
+      <c r="A21" s="41" t="n">
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="44" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -2751,10 +2755,10 @@
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="44" t="s">
+      <c r="I21" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="45" t="n">
+      <c r="J21" s="46" t="n">
         <v>4607174577787</v>
       </c>
       <c r="K21" s="16"/>
@@ -2780,7 +2784,7 @@
       <c r="U21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V21" s="46" t="n">
+      <c r="V21" s="47" t="n">
         <v>0.02</v>
       </c>
       <c r="W21" s="3"/>
@@ -2792,22 +2796,22 @@
         <v>3</v>
       </c>
       <c r="AC21" s="6"/>
-      <c r="AD21" s="41" t="s">
+      <c r="AD21" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="40" t="n">
+      <c r="A22" s="41" t="n">
         <v>20</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="50" t="s">
         <v>93</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -2838,10 +2842,10 @@
       <c r="T22" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="U22" s="41" t="s">
+      <c r="U22" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="V22" s="46" t="n">
+      <c r="V22" s="47" t="n">
         <v>0.1</v>
       </c>
       <c r="W22" s="3"/>
@@ -2857,16 +2861,16 @@
       <c r="AE22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="40" t="n">
+      <c r="A23" s="41" t="n">
         <v>21</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="50" t="s">
         <v>98</v>
       </c>
       <c r="E23" s="11" t="s">
@@ -2878,7 +2882,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="11"/>
-      <c r="J23" s="50" t="n">
+      <c r="J23" s="51" t="n">
         <v>22</v>
       </c>
       <c r="K23" s="5"/>
@@ -2897,10 +2901,10 @@
       <c r="T23" s="11" t="n">
         <v>21</v>
       </c>
-      <c r="U23" s="41" t="s">
+      <c r="U23" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="V23" s="46" t="n">
+      <c r="V23" s="47" t="n">
         <v>0.1</v>
       </c>
       <c r="W23" s="3"/>
@@ -2916,16 +2920,16 @@
       <c r="AE23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="40" t="n">
+      <c r="A24" s="41" t="n">
         <v>22</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="51" t="s">
+      <c r="D24" s="52" t="s">
         <v>100</v>
       </c>
       <c r="E24" s="11" t="s">
@@ -2937,7 +2941,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="11"/>
-      <c r="J24" s="50" t="n">
+      <c r="J24" s="51" t="n">
         <v>23</v>
       </c>
       <c r="K24" s="5"/>
@@ -2956,10 +2960,10 @@
       <c r="T24" s="11" t="n">
         <v>22</v>
       </c>
-      <c r="U24" s="41" t="s">
+      <c r="U24" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="46" t="n">
+      <c r="V24" s="47" t="n">
         <v>0.1</v>
       </c>
       <c r="W24" s="3"/>
@@ -2994,26 +2998,26 @@
   </sheetPr>
   <dimension ref="A1:AF34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="53.668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="53" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="53" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="28.1740890688259"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="54" width="66.1983805668016"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="55" width="66.8421052631579"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="24" min="16" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="27" min="26" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="53" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="54" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3027,7 +3031,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="56" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -3045,7 +3049,7 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="J1" s="57" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -3099,7 +3103,7 @@
       <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="57" t="s">
+      <c r="AB1" s="58" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="13" t="s">
@@ -3113,7 +3117,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="55" t="n">
+      <c r="A2" s="56" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -3122,7 +3126,7 @@
       <c r="C2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="59" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -3132,7 +3136,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="56"/>
+      <c r="J2" s="57"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="3"/>
@@ -3156,7 +3160,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
-      <c r="AB2" s="57" t="n">
+      <c r="AB2" s="58" t="n">
         <v>2</v>
       </c>
       <c r="AC2" s="13" t="s">
@@ -3166,7 +3170,7 @@
       <c r="AE2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="55" t="n">
+      <c r="A3" s="56" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -3175,10 +3179,10 @@
       <c r="C3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="19" t="n">
@@ -3189,7 +3193,7 @@
       <c r="I3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="61" t="n">
+      <c r="J3" s="62" t="n">
         <v>54491472</v>
       </c>
       <c r="K3" s="16"/>
@@ -3213,15 +3217,15 @@
       <c r="U3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V3" s="17" t="n">
-        <v>0.0286</v>
+      <c r="V3" s="63" t="n">
+        <v>0.028568</v>
       </c>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="57" t="n">
+      <c r="AB3" s="58" t="n">
         <v>3</v>
       </c>
       <c r="AC3" s="6"/>
@@ -3231,7 +3235,7 @@
       <c r="AE3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="55" t="n">
+      <c r="A4" s="56" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -3240,10 +3244,10 @@
       <c r="C4" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="19" t="n">
@@ -3254,7 +3258,7 @@
       <c r="I4" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="61" t="n">
+      <c r="J4" s="62" t="n">
         <v>5449000131836</v>
       </c>
       <c r="K4" s="16"/>
@@ -3278,15 +3282,15 @@
       <c r="U4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="17" t="n">
-        <v>0.0286</v>
+      <c r="V4" s="63" t="n">
+        <v>0.028572</v>
       </c>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="57" t="n">
+      <c r="AB4" s="58" t="n">
         <v>3</v>
       </c>
       <c r="AC4" s="6"/>
@@ -3296,7 +3300,7 @@
       <c r="AE4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="55" t="n">
+      <c r="A5" s="56" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -3305,10 +3309,10 @@
       <c r="C5" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="19" t="n">
@@ -3319,7 +3323,7 @@
       <c r="I5" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="61" t="n">
+      <c r="J5" s="62" t="n">
         <v>40822938</v>
       </c>
       <c r="K5" s="16"/>
@@ -3343,15 +3347,15 @@
       <c r="U5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="17" t="n">
-        <v>0.0286</v>
+      <c r="V5" s="63" t="n">
+        <v>0.028572</v>
       </c>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="57" t="n">
+      <c r="AB5" s="58" t="n">
         <v>3</v>
       </c>
       <c r="AC5" s="6"/>
@@ -3361,7 +3365,7 @@
       <c r="AE5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="55" t="n">
+      <c r="A6" s="56" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -3370,10 +3374,10 @@
       <c r="C6" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="19" t="n">
@@ -3384,7 +3388,7 @@
       <c r="I6" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="61" t="n">
+      <c r="J6" s="62" t="n">
         <v>54491069</v>
       </c>
       <c r="K6" s="16"/>
@@ -3408,15 +3412,15 @@
       <c r="U6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V6" s="17" t="n">
-        <v>0.0286</v>
+      <c r="V6" s="63" t="n">
+        <v>0.028572</v>
       </c>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="57" t="n">
+      <c r="AB6" s="58" t="n">
         <v>3</v>
       </c>
       <c r="AC6" s="6"/>
@@ -3426,7 +3430,7 @@
       <c r="AE6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="55" t="n">
+      <c r="A7" s="56" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -3435,10 +3439,10 @@
       <c r="C7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="19" t="n">
@@ -3473,15 +3477,15 @@
       <c r="U7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V7" s="17" t="n">
-        <v>0.0286</v>
+      <c r="V7" s="63" t="n">
+        <v>0.028572</v>
       </c>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="57" t="n">
+      <c r="AB7" s="58" t="n">
         <v>3</v>
       </c>
       <c r="AC7" s="6"/>
@@ -3491,7 +3495,7 @@
       <c r="AE7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="55" t="n">
+      <c r="A8" s="56" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -3500,10 +3504,10 @@
       <c r="C8" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="19" t="n">
@@ -3514,7 +3518,7 @@
       <c r="I8" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="61" t="n">
+      <c r="J8" s="62" t="n">
         <v>5449000189301</v>
       </c>
       <c r="K8" s="16"/>
@@ -3538,15 +3542,15 @@
       <c r="U8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V8" s="17" t="n">
-        <v>0.0286</v>
+      <c r="V8" s="63" t="n">
+        <v>0.028572</v>
       </c>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="57" t="n">
+      <c r="AB8" s="58" t="n">
         <v>3</v>
       </c>
       <c r="AC8" s="6"/>
@@ -3556,30 +3560,30 @@
       <c r="AE8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="55" t="n">
+      <c r="A9" s="56" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="19" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="19"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63" t="s">
+      <c r="H9" s="65"/>
+      <c r="I9" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="61" t="n">
+      <c r="J9" s="62" t="n">
         <v>4607174577787</v>
       </c>
       <c r="K9" s="5"/>
@@ -3603,15 +3607,15 @@
       <c r="U9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V9" s="17" t="n">
-        <v>0.0286</v>
+      <c r="V9" s="63" t="n">
+        <v>0.028572</v>
       </c>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="57" t="n">
+      <c r="AB9" s="58" t="n">
         <v>3</v>
       </c>
       <c r="AC9" s="13"/>
@@ -3621,16 +3625,16 @@
       <c r="AE9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="55" t="n">
+      <c r="A10" s="56" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="60" t="s">
         <v>58</v>
       </c>
       <c r="E10" s="10" t="s">
@@ -3640,11 +3644,11 @@
         <v>22</v>
       </c>
       <c r="G10" s="19"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63" t="s">
+      <c r="H10" s="65"/>
+      <c r="I10" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="64" t="s">
+      <c r="J10" s="66" t="s">
         <v>60</v>
       </c>
       <c r="K10" s="5"/>
@@ -3668,7 +3672,7 @@
       <c r="U10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="V10" s="17" t="n">
+      <c r="V10" s="24" t="n">
         <v>0.2</v>
       </c>
       <c r="W10" s="3"/>
@@ -3676,7 +3680,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="57" t="n">
+      <c r="AB10" s="58" t="n">
         <v>2</v>
       </c>
       <c r="AC10" s="13"/>
@@ -3684,26 +3688,26 @@
       <c r="AE10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="64.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="55" t="n">
+      <c r="A11" s="56" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="65" t="s">
+      <c r="E11" s="67" t="s">
         <v>64</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="56"/>
+      <c r="J11" s="57"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="3"/>
@@ -3719,15 +3723,15 @@
       <c r="U11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V11" s="42"/>
+      <c r="V11" s="43"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="66" t="s">
+      <c r="Y11" s="68" t="s">
         <v>66</v>
       </c>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="57" t="n">
+      <c r="AB11" s="58" t="n">
         <v>2</v>
       </c>
       <c r="AC11" s="13" t="s">
@@ -3737,16 +3741,16 @@
       <c r="AE11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="69.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="55" t="n">
+      <c r="A12" s="56" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="42" t="s">
         <v>108</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -3756,12 +3760,12 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="56"/>
+      <c r="J12" s="57"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="67" t="s">
+      <c r="O12" s="69" t="s">
         <v>109</v>
       </c>
       <c r="P12" s="3"/>
@@ -3774,896 +3778,896 @@
       <c r="U12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V12" s="68" t="n">
+      <c r="V12" s="70" t="n">
         <f aca="false">SUM(V13:V18)</f>
-        <v>0.033329</v>
+        <v>0.033364</v>
       </c>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
-      <c r="Y12" s="69" t="s">
+      <c r="Y12" s="71" t="s">
         <v>110</v>
       </c>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="57" t="n">
+      <c r="AB12" s="58" t="n">
         <v>3</v>
       </c>
       <c r="AC12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="AD12" s="41" t="s">
+      <c r="AD12" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" s="80" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="55" t="n">
+    <row r="13" s="81" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="56" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="60" t="s">
+      <c r="E13" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="60" t="n">
+      <c r="F13" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
       <c r="I13" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="61" t="n">
+      <c r="J13" s="62" t="n">
         <v>54491472</v>
       </c>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="67" t="s">
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="67" t="s">
+      <c r="N13" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O13" s="74" t="s">
+      <c r="O13" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="67"/>
-      <c r="R13" s="67"/>
-      <c r="S13" s="67" t="n">
+      <c r="P13" s="69"/>
+      <c r="Q13" s="69"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="T13" s="67" t="n">
+      <c r="T13" s="69" t="n">
         <v>12</v>
       </c>
-      <c r="U13" s="67" t="s">
+      <c r="U13" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V13" s="75" t="n">
+      <c r="V13" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W13" s="67"/>
-      <c r="X13" s="67"/>
-      <c r="Y13" s="67"/>
-      <c r="Z13" s="67"/>
-      <c r="AA13" s="67"/>
-      <c r="AB13" s="76" t="n">
+      <c r="W13" s="69"/>
+      <c r="X13" s="69"/>
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC13" s="77"/>
-      <c r="AD13" s="78" t="s">
+      <c r="AC13" s="78"/>
+      <c r="AD13" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="AE13" s="79"/>
-    </row>
-    <row r="14" s="80" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55" t="n">
+      <c r="AE13" s="80"/>
+    </row>
+    <row r="14" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="56" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="73" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="72" t="s">
+      <c r="D14" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="60" t="s">
+      <c r="E14" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="60" t="n">
+      <c r="F14" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
       <c r="I14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="61" t="n">
+      <c r="J14" s="62" t="n">
         <v>54491472</v>
       </c>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="67" t="s">
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N14" s="67" t="s">
+      <c r="N14" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O14" s="67" t="s">
+      <c r="O14" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="67"/>
-      <c r="S14" s="67" t="n">
+      <c r="P14" s="69"/>
+      <c r="Q14" s="69"/>
+      <c r="R14" s="69"/>
+      <c r="S14" s="69" t="n">
         <v>2</v>
       </c>
-      <c r="T14" s="67" t="n">
+      <c r="T14" s="69" t="n">
         <v>13</v>
       </c>
-      <c r="U14" s="67" t="s">
+      <c r="U14" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V14" s="75" t="n">
+      <c r="V14" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W14" s="67"/>
-      <c r="X14" s="67"/>
-      <c r="Y14" s="67"/>
-      <c r="Z14" s="67"/>
-      <c r="AA14" s="67"/>
-      <c r="AB14" s="76" t="n">
+      <c r="W14" s="69"/>
+      <c r="X14" s="69"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC14" s="77"/>
-      <c r="AD14" s="78" t="s">
+      <c r="AC14" s="78"/>
+      <c r="AD14" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="AE14" s="79"/>
-    </row>
-    <row r="15" s="80" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="55" t="n">
+      <c r="AE14" s="80"/>
+    </row>
+    <row r="15" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="56" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="60" t="n">
+      <c r="F15" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
       <c r="I15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="61" t="n">
+      <c r="J15" s="62" t="n">
         <v>5449000131836</v>
       </c>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="67" t="s">
+      <c r="K15" s="75"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N15" s="67" t="s">
+      <c r="N15" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="67" t="s">
+      <c r="O15" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="67"/>
-      <c r="R15" s="67"/>
-      <c r="S15" s="67" t="n">
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69" t="n">
         <v>3</v>
       </c>
-      <c r="T15" s="67" t="n">
+      <c r="T15" s="69" t="n">
         <v>14</v>
       </c>
-      <c r="U15" s="67" t="s">
+      <c r="U15" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V15" s="75" t="n">
+      <c r="V15" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W15" s="67"/>
-      <c r="X15" s="67"/>
-      <c r="Y15" s="67"/>
-      <c r="Z15" s="67"/>
-      <c r="AA15" s="67"/>
-      <c r="AB15" s="76" t="n">
+      <c r="W15" s="69"/>
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC15" s="77"/>
-      <c r="AD15" s="78" t="s">
+      <c r="AC15" s="78"/>
+      <c r="AD15" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="AE15" s="79"/>
-    </row>
-    <row r="16" s="80" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="55" t="n">
+      <c r="AE15" s="80"/>
+    </row>
+    <row r="16" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="56" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="72" t="s">
+      <c r="D16" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="60" t="s">
+      <c r="E16" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="60" t="n">
+      <c r="F16" s="61" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
       <c r="I16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="61" t="n">
+      <c r="J16" s="62" t="n">
         <v>40822938</v>
       </c>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="67" t="s">
+      <c r="K16" s="75"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="67" t="s">
+      <c r="N16" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="67" t="s">
+      <c r="O16" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="67"/>
-      <c r="R16" s="67"/>
-      <c r="S16" s="67" t="n">
+      <c r="P16" s="69"/>
+      <c r="Q16" s="69"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="69" t="n">
         <v>4</v>
       </c>
-      <c r="T16" s="67" t="n">
+      <c r="T16" s="69" t="n">
         <v>15</v>
       </c>
-      <c r="U16" s="67" t="s">
+      <c r="U16" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V16" s="75" t="n">
-        <v>0.002962</v>
-      </c>
-      <c r="W16" s="67"/>
-      <c r="X16" s="67"/>
-      <c r="Y16" s="67"/>
-      <c r="Z16" s="67"/>
-      <c r="AA16" s="67"/>
-      <c r="AB16" s="76" t="n">
+      <c r="V16" s="82" t="n">
+        <v>0.0031</v>
+      </c>
+      <c r="W16" s="69"/>
+      <c r="X16" s="69"/>
+      <c r="Y16" s="69"/>
+      <c r="Z16" s="69"/>
+      <c r="AA16" s="69"/>
+      <c r="AB16" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC16" s="77"/>
-      <c r="AD16" s="78" t="s">
+      <c r="AC16" s="78"/>
+      <c r="AD16" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="AE16" s="79"/>
-    </row>
-    <row r="17" s="80" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="55" t="n">
+      <c r="AE16" s="80"/>
+    </row>
+    <row r="17" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="56" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="72" t="s">
+      <c r="D17" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="60" t="n">
+      <c r="F17" s="61" t="n">
         <v>4</v>
       </c>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
       <c r="I17" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="61" t="n">
+      <c r="J17" s="62" t="n">
         <v>54491069</v>
       </c>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="67" t="s">
+      <c r="K17" s="75"/>
+      <c r="L17" s="75"/>
+      <c r="M17" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="67" t="s">
+      <c r="N17" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O17" s="67" t="s">
+      <c r="O17" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P17" s="67"/>
-      <c r="Q17" s="67"/>
-      <c r="R17" s="67"/>
-      <c r="S17" s="67" t="n">
+      <c r="P17" s="69"/>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="69" t="n">
         <v>4</v>
       </c>
-      <c r="T17" s="67" t="n">
+      <c r="T17" s="69" t="n">
         <v>16</v>
       </c>
-      <c r="U17" s="67" t="s">
+      <c r="U17" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V17" s="75" t="n">
-        <v>0.003703</v>
-      </c>
-      <c r="W17" s="67"/>
-      <c r="X17" s="67"/>
-      <c r="Y17" s="67"/>
-      <c r="Z17" s="67"/>
-      <c r="AA17" s="67"/>
-      <c r="AB17" s="76" t="n">
+      <c r="V17" s="82" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="W17" s="69"/>
+      <c r="X17" s="69"/>
+      <c r="Y17" s="69"/>
+      <c r="Z17" s="69"/>
+      <c r="AA17" s="69"/>
+      <c r="AB17" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC17" s="77"/>
-      <c r="AD17" s="78" t="s">
+      <c r="AC17" s="78"/>
+      <c r="AD17" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="AE17" s="79"/>
-    </row>
-    <row r="18" s="80" customFormat="true" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="55" t="n">
+      <c r="AE17" s="80"/>
+    </row>
+    <row r="18" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="56" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="60" t="n">
+      <c r="F18" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
       <c r="I18" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="61" t="n">
+      <c r="J18" s="62" t="n">
         <v>54491472</v>
       </c>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="67" t="s">
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N18" s="67" t="s">
+      <c r="N18" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O18" s="67" t="s">
+      <c r="O18" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="67"/>
-      <c r="R18" s="67"/>
-      <c r="S18" s="67" t="n">
+      <c r="P18" s="69"/>
+      <c r="Q18" s="69"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="69" t="n">
         <v>5</v>
       </c>
-      <c r="T18" s="67" t="n">
+      <c r="T18" s="69" t="n">
         <v>17</v>
       </c>
-      <c r="U18" s="67" t="s">
+      <c r="U18" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V18" s="75" t="n">
+      <c r="V18" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W18" s="67"/>
-      <c r="X18" s="67"/>
-      <c r="Y18" s="67"/>
-      <c r="Z18" s="67"/>
-      <c r="AA18" s="67"/>
-      <c r="AB18" s="76" t="n">
+      <c r="W18" s="69"/>
+      <c r="X18" s="69"/>
+      <c r="Y18" s="69"/>
+      <c r="Z18" s="69"/>
+      <c r="AA18" s="69"/>
+      <c r="AB18" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC18" s="77"/>
-      <c r="AD18" s="78" t="s">
+      <c r="AC18" s="78"/>
+      <c r="AD18" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="AE18" s="79"/>
+      <c r="AE18" s="80"/>
     </row>
     <row r="19" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="55" t="n">
+      <c r="A19" s="56" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="74" t="s">
         <v>124</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
       <c r="I19" s="20"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="67" t="s">
+      <c r="J19" s="62"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N19" s="67"/>
-      <c r="O19" s="67" t="s">
+      <c r="N19" s="69"/>
+      <c r="O19" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="P19" s="67"/>
-      <c r="Q19" s="67"/>
-      <c r="R19" s="67"/>
-      <c r="S19" s="67"/>
-      <c r="T19" s="67" t="n">
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="69" t="n">
         <v>18</v>
       </c>
       <c r="U19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V19" s="68" t="n">
+      <c r="V19" s="70" t="n">
         <f aca="false">SUM(V20:V24)</f>
         <v>0.03333</v>
       </c>
-      <c r="W19" s="67"/>
-      <c r="X19" s="67"/>
-      <c r="Y19" s="69" t="s">
+      <c r="W19" s="69"/>
+      <c r="X19" s="69"/>
+      <c r="Y19" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="Z19" s="67"/>
-      <c r="AA19" s="67"/>
-      <c r="AB19" s="76" t="n">
+      <c r="Z19" s="69"/>
+      <c r="AA19" s="69"/>
+      <c r="AB19" s="77" t="n">
         <v>3</v>
       </c>
-      <c r="AC19" s="81" t="s">
+      <c r="AC19" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="AD19" s="78"/>
-      <c r="AE19" s="79"/>
+      <c r="AD19" s="79"/>
+      <c r="AE19" s="80"/>
     </row>
     <row r="20" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="55" t="n">
+      <c r="A20" s="56" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="72" t="s">
+      <c r="D20" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="60" t="n">
+      <c r="F20" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
       <c r="I20" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="82" t="n">
+      <c r="J20" s="84" t="n">
         <v>5449000189301</v>
       </c>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="67" t="s">
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N20" s="67" t="s">
+      <c r="N20" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O20" s="67" t="s">
+      <c r="O20" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="67"/>
-      <c r="R20" s="67"/>
-      <c r="S20" s="67" t="n">
+      <c r="P20" s="69"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="T20" s="67" t="n">
+      <c r="T20" s="69" t="n">
         <v>19</v>
       </c>
-      <c r="U20" s="67" t="s">
+      <c r="U20" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V20" s="75" t="n">
+      <c r="V20" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W20" s="67"/>
-      <c r="X20" s="67"/>
-      <c r="Y20" s="67"/>
-      <c r="Z20" s="67"/>
-      <c r="AA20" s="67"/>
-      <c r="AB20" s="76" t="n">
+      <c r="W20" s="69"/>
+      <c r="X20" s="69"/>
+      <c r="Y20" s="69"/>
+      <c r="Z20" s="69"/>
+      <c r="AA20" s="69"/>
+      <c r="AB20" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC20" s="83"/>
-      <c r="AD20" s="78" t="s">
+      <c r="AC20" s="85"/>
+      <c r="AD20" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="AE20" s="79"/>
+      <c r="AE20" s="80"/>
     </row>
     <row r="21" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="55" t="n">
+      <c r="A21" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="E21" s="60" t="s">
+      <c r="E21" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="60" t="n">
+      <c r="F21" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
       <c r="I21" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="82" t="n">
+      <c r="J21" s="84" t="n">
         <v>5449000189301</v>
       </c>
-      <c r="K21" s="73"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="67" t="s">
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
+      <c r="M21" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N21" s="67" t="s">
+      <c r="N21" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O21" s="67" t="s">
+      <c r="O21" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="P21" s="67"/>
-      <c r="Q21" s="67"/>
-      <c r="R21" s="67"/>
-      <c r="S21" s="67" t="n">
+      <c r="P21" s="69"/>
+      <c r="Q21" s="69"/>
+      <c r="R21" s="69"/>
+      <c r="S21" s="69" t="n">
         <v>2</v>
       </c>
-      <c r="T21" s="67" t="n">
+      <c r="T21" s="69" t="n">
         <v>20</v>
       </c>
-      <c r="U21" s="67" t="s">
+      <c r="U21" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V21" s="75" t="n">
+      <c r="V21" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W21" s="67"/>
-      <c r="X21" s="67"/>
-      <c r="Y21" s="67"/>
-      <c r="Z21" s="67"/>
-      <c r="AA21" s="67"/>
-      <c r="AB21" s="76" t="n">
+      <c r="W21" s="69"/>
+      <c r="X21" s="69"/>
+      <c r="Y21" s="69"/>
+      <c r="Z21" s="69"/>
+      <c r="AA21" s="69"/>
+      <c r="AB21" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC21" s="83"/>
-      <c r="AD21" s="78" t="s">
+      <c r="AC21" s="85"/>
+      <c r="AD21" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="AE21" s="79"/>
+      <c r="AE21" s="80"/>
     </row>
     <row r="22" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="55" t="n">
+      <c r="A22" s="56" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="84" t="s">
+      <c r="D22" s="86" t="s">
         <v>132</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="60" t="n">
+      <c r="F22" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
       <c r="I22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J22" s="85" t="n">
+      <c r="J22" s="87" t="n">
         <v>4607174577787</v>
       </c>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="67" t="s">
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N22" s="67" t="s">
+      <c r="N22" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O22" s="67" t="s">
+      <c r="O22" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="67" t="n">
+      <c r="P22" s="69"/>
+      <c r="Q22" s="69"/>
+      <c r="R22" s="69"/>
+      <c r="S22" s="69" t="n">
         <v>3</v>
       </c>
-      <c r="T22" s="67" t="n">
+      <c r="T22" s="69" t="n">
         <v>21</v>
       </c>
-      <c r="U22" s="67" t="s">
+      <c r="U22" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V22" s="75" t="n">
+      <c r="V22" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W22" s="67"/>
-      <c r="X22" s="67"/>
-      <c r="Y22" s="67"/>
-      <c r="Z22" s="67"/>
-      <c r="AA22" s="67"/>
-      <c r="AB22" s="76" t="n">
+      <c r="W22" s="69"/>
+      <c r="X22" s="69"/>
+      <c r="Y22" s="69"/>
+      <c r="Z22" s="69"/>
+      <c r="AA22" s="69"/>
+      <c r="AB22" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC22" s="83"/>
-      <c r="AD22" s="78" t="s">
+      <c r="AC22" s="85"/>
+      <c r="AD22" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="AE22" s="79"/>
+      <c r="AE22" s="80"/>
     </row>
     <row r="23" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="55" t="n">
+      <c r="A23" s="56" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="84" t="s">
+      <c r="D23" s="86" t="s">
         <v>134</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="60" t="n">
+      <c r="F23" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
       <c r="I23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="85" t="n">
+      <c r="J23" s="87" t="n">
         <v>4607174577787</v>
       </c>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="67" t="s">
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N23" s="67" t="s">
+      <c r="N23" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O23" s="67" t="s">
+      <c r="O23" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="P23" s="67"/>
-      <c r="Q23" s="67"/>
-      <c r="R23" s="67"/>
-      <c r="S23" s="67" t="n">
+      <c r="P23" s="69"/>
+      <c r="Q23" s="69"/>
+      <c r="R23" s="69"/>
+      <c r="S23" s="69" t="n">
         <v>4</v>
       </c>
-      <c r="T23" s="67" t="n">
+      <c r="T23" s="69" t="n">
         <v>22</v>
       </c>
-      <c r="U23" s="67" t="s">
+      <c r="U23" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V23" s="75" t="n">
+      <c r="V23" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W23" s="67"/>
-      <c r="X23" s="67"/>
-      <c r="Y23" s="67"/>
-      <c r="Z23" s="67"/>
-      <c r="AA23" s="67"/>
-      <c r="AB23" s="76" t="n">
+      <c r="W23" s="69"/>
+      <c r="X23" s="69"/>
+      <c r="Y23" s="69"/>
+      <c r="Z23" s="69"/>
+      <c r="AA23" s="69"/>
+      <c r="AB23" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC23" s="83"/>
-      <c r="AD23" s="78" t="s">
+      <c r="AC23" s="85"/>
+      <c r="AD23" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="AE23" s="79"/>
+      <c r="AE23" s="80"/>
     </row>
     <row r="24" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="55" t="n">
+      <c r="A24" s="56" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="71" t="s">
+      <c r="C24" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="72" t="s">
+      <c r="D24" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="60" t="n">
+      <c r="F24" s="61" t="n">
         <v>7</v>
       </c>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
       <c r="I24" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="61" t="n">
+      <c r="J24" s="62" t="n">
         <v>54491472</v>
       </c>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="67" t="s">
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N24" s="67" t="s">
+      <c r="N24" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O24" s="67" t="s">
+      <c r="O24" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="67"/>
-      <c r="S24" s="67" t="n">
+      <c r="P24" s="69"/>
+      <c r="Q24" s="69"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="69" t="n">
         <v>5</v>
       </c>
-      <c r="T24" s="67" t="n">
+      <c r="T24" s="69" t="n">
         <v>23</v>
       </c>
-      <c r="U24" s="67" t="s">
+      <c r="U24" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="75" t="n">
+      <c r="V24" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W24" s="67"/>
-      <c r="X24" s="67"/>
-      <c r="Y24" s="67"/>
-      <c r="Z24" s="67"/>
-      <c r="AA24" s="67"/>
-      <c r="AB24" s="76" t="n">
+      <c r="W24" s="69"/>
+      <c r="X24" s="69"/>
+      <c r="Y24" s="69"/>
+      <c r="Z24" s="69"/>
+      <c r="AA24" s="69"/>
+      <c r="AB24" s="77" t="n">
         <v>4</v>
       </c>
-      <c r="AC24" s="83"/>
-      <c r="AD24" s="78" t="s">
+      <c r="AC24" s="85"/>
+      <c r="AD24" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="AE24" s="79"/>
+      <c r="AE24" s="80"/>
     </row>
     <row r="25" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="55" t="n">
+      <c r="A25" s="56" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="70" t="s">
+      <c r="B25" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="72" t="s">
+      <c r="D25" s="74" t="s">
         <v>137</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
       <c r="I25" s="20"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="67" t="s">
+      <c r="J25" s="62"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="75"/>
+      <c r="M25" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67" t="s">
+      <c r="N25" s="69"/>
+      <c r="O25" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="67"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="67" t="n">
+      <c r="P25" s="69"/>
+      <c r="Q25" s="69"/>
+      <c r="R25" s="69"/>
+      <c r="S25" s="85"/>
+      <c r="T25" s="69" t="n">
         <v>24</v>
       </c>
       <c r="U25" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V25" s="68" t="n">
+      <c r="V25" s="70" t="n">
         <f aca="false">SUM(V26:V30)</f>
         <v>0.03333</v>
       </c>
-      <c r="W25" s="67"/>
-      <c r="X25" s="67"/>
-      <c r="Y25" s="69" t="s">
+      <c r="W25" s="69"/>
+      <c r="X25" s="69"/>
+      <c r="Y25" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="Z25" s="67"/>
-      <c r="AA25" s="67"/>
-      <c r="AB25" s="76" t="n">
+      <c r="Z25" s="69"/>
+      <c r="AA25" s="69"/>
+      <c r="AB25" s="77" t="n">
         <v>3</v>
       </c>
-      <c r="AC25" s="81" t="s">
+      <c r="AC25" s="83" t="s">
         <v>139</v>
       </c>
-      <c r="AD25" s="78"/>
-      <c r="AE25" s="79"/>
+      <c r="AD25" s="79"/>
+      <c r="AE25" s="80"/>
     </row>
     <row r="26" s="4" customFormat="true" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="55" t="n">
+      <c r="A26" s="56" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="71" t="s">
+      <c r="C26" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="72" t="s">
+      <c r="D26" s="74" t="s">
         <v>141</v>
       </c>
       <c r="E26" s="11" t="s">
@@ -4688,22 +4692,22 @@
       <c r="N26" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O26" s="67" t="s">
+      <c r="O26" s="69" t="s">
         <v>138</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
       <c r="R26" s="11"/>
-      <c r="S26" s="67" t="n">
+      <c r="S26" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="T26" s="67" t="n">
+      <c r="T26" s="69" t="n">
         <v>25</v>
       </c>
-      <c r="U26" s="67" t="s">
+      <c r="U26" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V26" s="75" t="n">
+      <c r="V26" s="76" t="n">
         <v>0.006666</v>
       </c>
       <c r="W26" s="3"/>
@@ -4711,26 +4715,26 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
-      <c r="AB26" s="57" t="n">
+      <c r="AB26" s="58" t="n">
         <v>4</v>
       </c>
       <c r="AC26" s="6"/>
-      <c r="AD26" s="78" t="s">
+      <c r="AD26" s="79" t="s">
         <v>136</v>
       </c>
       <c r="AE26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="55" t="n">
+      <c r="A27" s="56" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="88" t="s">
         <v>143</v>
       </c>
       <c r="E27" s="11" t="s">
@@ -4755,22 +4759,22 @@
       <c r="N27" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O27" s="67" t="s">
+      <c r="O27" s="69" t="s">
         <v>138</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
       <c r="R27" s="11"/>
-      <c r="S27" s="67" t="n">
+      <c r="S27" s="69" t="n">
         <v>2</v>
       </c>
-      <c r="T27" s="67" t="n">
+      <c r="T27" s="69" t="n">
         <v>26</v>
       </c>
-      <c r="U27" s="67" t="s">
+      <c r="U27" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V27" s="75" t="n">
+      <c r="V27" s="76" t="n">
         <v>0.006666</v>
       </c>
       <c r="W27" s="3"/>
@@ -4778,26 +4782,26 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
-      <c r="AB27" s="57" t="n">
+      <c r="AB27" s="58" t="n">
         <v>4</v>
       </c>
       <c r="AC27" s="6"/>
-      <c r="AD27" s="78" t="s">
+      <c r="AD27" s="79" t="s">
         <v>136</v>
       </c>
       <c r="AE27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="55" t="n">
+      <c r="A28" s="56" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="86" t="s">
+      <c r="D28" s="88" t="s">
         <v>145</v>
       </c>
       <c r="E28" s="11" t="s">
@@ -4822,22 +4826,22 @@
       <c r="N28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O28" s="67" t="s">
+      <c r="O28" s="69" t="s">
         <v>138</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
       <c r="R28" s="11"/>
-      <c r="S28" s="67" t="n">
+      <c r="S28" s="69" t="n">
         <v>3</v>
       </c>
-      <c r="T28" s="67" t="n">
+      <c r="T28" s="69" t="n">
         <v>27</v>
       </c>
-      <c r="U28" s="67" t="s">
+      <c r="U28" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V28" s="75" t="n">
+      <c r="V28" s="76" t="n">
         <v>0.006666</v>
       </c>
       <c r="W28" s="3"/>
@@ -4845,26 +4849,26 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
-      <c r="AB28" s="57" t="n">
+      <c r="AB28" s="58" t="n">
         <v>4</v>
       </c>
       <c r="AC28" s="6"/>
-      <c r="AD28" s="78" t="s">
+      <c r="AD28" s="79" t="s">
         <v>136</v>
       </c>
       <c r="AE28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="55" t="n">
+      <c r="A29" s="56" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="86" t="s">
+      <c r="D29" s="88" t="s">
         <v>147</v>
       </c>
       <c r="E29" s="11" t="s">
@@ -4881,7 +4885,7 @@
       <c r="J29" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K29" s="83"/>
+      <c r="K29" s="85"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5" t="s">
         <v>40</v>
@@ -4889,50 +4893,50 @@
       <c r="N29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O29" s="67" t="s">
+      <c r="O29" s="69" t="s">
         <v>138</v>
       </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="67" t="n">
+      <c r="S29" s="69" t="n">
         <v>4</v>
       </c>
-      <c r="T29" s="67" t="n">
+      <c r="T29" s="69" t="n">
         <v>28</v>
       </c>
-      <c r="U29" s="67" t="s">
+      <c r="U29" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V29" s="75" t="n">
+      <c r="V29" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W29" s="46"/>
+      <c r="W29" s="47"/>
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
-      <c r="AB29" s="57" t="n">
+      <c r="AB29" s="58" t="n">
         <v>4</v>
       </c>
       <c r="AC29" s="6"/>
-      <c r="AD29" s="78" t="s">
+      <c r="AD29" s="79" t="s">
         <v>136</v>
       </c>
       <c r="AE29" s="13"/>
-      <c r="AF29" s="87"/>
+      <c r="AF29" s="89"/>
     </row>
     <row r="30" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="55" t="n">
+      <c r="A30" s="56" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="D30" s="86" t="s">
+      <c r="D30" s="88" t="s">
         <v>149</v>
       </c>
       <c r="E30" s="11" t="s">
@@ -4949,7 +4953,7 @@
       <c r="J30" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K30" s="83"/>
+      <c r="K30" s="85"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5" t="s">
         <v>40</v>
@@ -4957,50 +4961,50 @@
       <c r="N30" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O30" s="67" t="s">
+      <c r="O30" s="69" t="s">
         <v>138</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="67" t="n">
+      <c r="S30" s="69" t="n">
         <v>5</v>
       </c>
-      <c r="T30" s="67" t="n">
+      <c r="T30" s="69" t="n">
         <v>29</v>
       </c>
-      <c r="U30" s="67" t="s">
+      <c r="U30" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="V30" s="75" t="n">
+      <c r="V30" s="76" t="n">
         <v>0.006666</v>
       </c>
-      <c r="W30" s="46"/>
+      <c r="W30" s="47"/>
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
       <c r="AA30" s="3"/>
-      <c r="AB30" s="57" t="n">
+      <c r="AB30" s="58" t="n">
         <v>4</v>
       </c>
       <c r="AC30" s="6"/>
-      <c r="AD30" s="78" t="s">
+      <c r="AD30" s="79" t="s">
         <v>136</v>
       </c>
       <c r="AE30" s="13"/>
-      <c r="AF30" s="88"/>
+      <c r="AF30" s="90"/>
     </row>
     <row r="31" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="55" t="n">
+      <c r="A31" s="56" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="D31" s="72" t="s">
+      <c r="D31" s="74" t="s">
         <v>151</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -5014,7 +5018,7 @@
       <c r="I31" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="J31" s="89" t="n">
+      <c r="J31" s="91" t="n">
         <v>1</v>
       </c>
       <c r="K31" s="5"/>
@@ -5029,14 +5033,14 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="67"/>
-      <c r="T31" s="67" t="n">
+      <c r="S31" s="69"/>
+      <c r="T31" s="69" t="n">
         <v>30</v>
       </c>
       <c r="U31" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V31" s="46" t="n">
+      <c r="V31" s="47" t="n">
         <v>0.2</v>
       </c>
       <c r="W31" s="3"/>
@@ -5044,25 +5048,25 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
       <c r="AA31" s="6"/>
-      <c r="AB31" s="57" t="n">
+      <c r="AB31" s="58" t="n">
         <v>2</v>
       </c>
       <c r="AC31" s="13"/>
-      <c r="AD31" s="78"/>
+      <c r="AD31" s="79"/>
       <c r="AE31" s="13"/>
-      <c r="AF31" s="88"/>
+      <c r="AF31" s="90"/>
     </row>
     <row r="32" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="55" t="n">
+      <c r="A32" s="56" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="D32" s="84" t="s">
+      <c r="D32" s="86" t="s">
         <v>154</v>
       </c>
       <c r="E32" s="11" t="s">
@@ -5076,7 +5080,7 @@
       <c r="I32" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="J32" s="82" t="n">
+      <c r="J32" s="84" t="n">
         <v>24</v>
       </c>
       <c r="K32" s="5"/>
@@ -5092,13 +5096,13 @@
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
-      <c r="T32" s="67" t="n">
+      <c r="T32" s="69" t="n">
         <v>31</v>
       </c>
       <c r="U32" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V32" s="46" t="n">
+      <c r="V32" s="47" t="n">
         <v>0.1</v>
       </c>
       <c r="W32" s="3"/>
@@ -5106,7 +5110,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
-      <c r="AB32" s="57" t="n">
+      <c r="AB32" s="58" t="n">
         <v>2</v>
       </c>
       <c r="AC32" s="2"/>
@@ -5114,16 +5118,16 @@
       <c r="AE32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="55" t="n">
+      <c r="A33" s="56" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="84" t="s">
+      <c r="D33" s="86" t="s">
         <v>100</v>
       </c>
       <c r="E33" s="11" t="s">
@@ -5137,7 +5141,7 @@
       <c r="I33" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="J33" s="82" t="n">
+      <c r="J33" s="84" t="n">
         <v>23</v>
       </c>
       <c r="K33" s="5"/>
@@ -5153,13 +5157,13 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
-      <c r="T33" s="67" t="n">
+      <c r="T33" s="69" t="n">
         <v>32</v>
       </c>
       <c r="U33" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V33" s="46" t="n">
+      <c r="V33" s="47" t="n">
         <v>0.1</v>
       </c>
       <c r="W33" s="3"/>
@@ -5167,7 +5171,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
-      <c r="AB33" s="57" t="n">
+      <c r="AB33" s="58" t="n">
         <v>2</v>
       </c>
       <c r="AC33" s="2"/>
@@ -5175,16 +5179,16 @@
       <c r="AE33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="55" t="n">
+      <c r="A34" s="56" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="42" t="s">
         <v>156</v>
       </c>
       <c r="E34" s="11" t="s">
@@ -5198,7 +5202,7 @@
       <c r="I34" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="J34" s="82" t="n">
+      <c r="J34" s="84" t="n">
         <v>16</v>
       </c>
       <c r="K34" s="5"/>
@@ -5214,13 +5218,13 @@
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
-      <c r="T34" s="67" t="n">
+      <c r="T34" s="69" t="n">
         <v>33</v>
       </c>
       <c r="U34" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V34" s="46" t="n">
+      <c r="V34" s="47" t="n">
         <v>0.1</v>
       </c>
       <c r="W34" s="3"/>
@@ -5228,7 +5232,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
-      <c r="AB34" s="57" t="n">
+      <c r="AB34" s="58" t="n">
         <v>2</v>
       </c>
       <c r="AC34" s="2"/>
@@ -5259,24 +5263,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="55" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="53" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="53" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="53" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="53" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="54" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="54" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="55" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="12" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.7449392712551"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="21" min="17" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="24" min="23" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="27" min="26" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="53" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="54" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5311,7 +5315,7 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="92" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -5362,7 +5366,7 @@
       <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="57" t="s">
+      <c r="AB1" s="58" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="7" t="s">
@@ -5376,34 +5380,34 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="91" t="n">
+      <c r="A2" s="93" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E2" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="94"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="94"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="96"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="98" t="s">
+      <c r="O2" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="98"/>
+      <c r="P2" s="100"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
@@ -5431,44 +5435,44 @@
       <c r="AF2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="91" t="n">
+      <c r="A3" s="93" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="99" t="s">
+      <c r="D3" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="100" t="s">
+      <c r="E3" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="100" t="n">
+      <c r="F3" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="95"/>
-      <c r="H3" s="101"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="103"/>
       <c r="I3" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="102" t="n">
+      <c r="J3" s="104" t="n">
         <v>54491472</v>
       </c>
-      <c r="K3" s="95"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103" t="s">
+      <c r="K3" s="97"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105" t="s">
         <v>40</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="98" t="s">
+      <c r="O3" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="98"/>
+      <c r="P3" s="100"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -5478,7 +5482,7 @@
       <c r="U3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V3" s="17" t="n">
+      <c r="V3" s="24" t="n">
         <v>0.04714</v>
       </c>
       <c r="X3" s="3"/>
@@ -5495,44 +5499,44 @@
       <c r="AF3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="91" t="n">
+      <c r="A4" s="93" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="99" t="s">
+      <c r="C4" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="100" t="s">
+      <c r="E4" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="100" t="n">
+      <c r="F4" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="95"/>
-      <c r="H4" s="101"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="103"/>
       <c r="I4" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="102" t="n">
+      <c r="J4" s="104" t="n">
         <v>5449000131836</v>
       </c>
-      <c r="K4" s="95"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103" t="s">
+      <c r="K4" s="97"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105" t="s">
         <v>40</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="98" t="s">
+      <c r="O4" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="98"/>
+      <c r="P4" s="100"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
@@ -5542,7 +5546,7 @@
       <c r="U4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="17" t="n">
+      <c r="V4" s="24" t="n">
         <v>0.04714</v>
       </c>
       <c r="X4" s="3"/>
@@ -5559,44 +5563,44 @@
       <c r="AF4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="91" t="n">
+      <c r="A5" s="93" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="99" t="s">
+      <c r="C5" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="99" t="s">
+      <c r="D5" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="100" t="s">
+      <c r="E5" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="100" t="n">
+      <c r="F5" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="95"/>
-      <c r="H5" s="101"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="103"/>
       <c r="I5" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="102" t="n">
+      <c r="J5" s="104" t="n">
         <v>40822938</v>
       </c>
-      <c r="K5" s="95"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103" t="s">
+      <c r="K5" s="97"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105" t="s">
         <v>40</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="98" t="s">
+      <c r="O5" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="98"/>
+      <c r="P5" s="100"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
@@ -5606,7 +5610,7 @@
       <c r="U5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="17" t="n">
+      <c r="V5" s="24" t="n">
         <v>0.04714</v>
       </c>
       <c r="X5" s="3"/>
@@ -5623,44 +5627,44 @@
       <c r="AF5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="91" t="n">
+      <c r="A6" s="93" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="99" t="s">
+      <c r="C6" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="99" t="s">
+      <c r="D6" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="100" t="s">
+      <c r="E6" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="100" t="n">
+      <c r="F6" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="95"/>
-      <c r="H6" s="101"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="103"/>
       <c r="I6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="102" t="n">
+      <c r="J6" s="104" t="n">
         <v>54491069</v>
       </c>
-      <c r="K6" s="95"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103" t="s">
+      <c r="K6" s="97"/>
+      <c r="L6" s="105"/>
+      <c r="M6" s="105" t="s">
         <v>40</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="98" t="s">
+      <c r="O6" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="98"/>
+      <c r="P6" s="100"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
       <c r="S6" s="11"/>
@@ -5670,7 +5674,7 @@
       <c r="U6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V6" s="17" t="n">
+      <c r="V6" s="24" t="n">
         <v>0.04714</v>
       </c>
       <c r="X6" s="3"/>
@@ -5687,44 +5691,44 @@
       <c r="AF6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="91" t="n">
+      <c r="A7" s="93" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="99" t="s">
+      <c r="C7" s="101" t="s">
         <v>158</v>
       </c>
-      <c r="D7" s="99" t="s">
+      <c r="D7" s="101" t="s">
         <v>159</v>
       </c>
-      <c r="E7" s="100" t="s">
+      <c r="E7" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="100" t="n">
+      <c r="F7" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="95"/>
-      <c r="H7" s="101"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="103"/>
       <c r="I7" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="J7" s="102" t="n">
+      <c r="J7" s="104" t="n">
         <v>40822426</v>
       </c>
-      <c r="K7" s="95"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103" t="s">
+      <c r="K7" s="97"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="105" t="s">
         <v>40</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="98" t="s">
+      <c r="O7" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="98"/>
+      <c r="P7" s="100"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -5734,7 +5738,7 @@
       <c r="U7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V7" s="17" t="n">
+      <c r="V7" s="24" t="n">
         <v>0.04714</v>
       </c>
       <c r="X7" s="3"/>
@@ -5751,44 +5755,44 @@
       <c r="AF7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="91" t="n">
+      <c r="A8" s="93" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C8" s="99" t="s">
+      <c r="C8" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="99" t="s">
+      <c r="D8" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="100" t="s">
+      <c r="E8" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="100" t="n">
+      <c r="F8" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="95"/>
-      <c r="H8" s="101"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="103"/>
       <c r="I8" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="102" t="n">
+      <c r="J8" s="104" t="n">
         <v>5449000189301</v>
       </c>
-      <c r="K8" s="95"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103" t="s">
+      <c r="K8" s="97"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105" t="s">
         <v>40</v>
       </c>
       <c r="N8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="98" t="s">
+      <c r="O8" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="98"/>
+      <c r="P8" s="100"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
@@ -5798,7 +5802,7 @@
       <c r="U8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V8" s="17" t="n">
+      <c r="V8" s="24" t="n">
         <v>0.04714</v>
       </c>
       <c r="X8" s="3"/>
@@ -5815,44 +5819,44 @@
       <c r="AF8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="91" t="n">
+      <c r="A9" s="93" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="104" t="s">
+      <c r="C9" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="99" t="s">
+      <c r="D9" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="100" t="s">
+      <c r="E9" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="100" t="n">
+      <c r="F9" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="95"/>
-      <c r="H9" s="101"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="103"/>
       <c r="I9" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="102" t="n">
+      <c r="J9" s="104" t="n">
         <v>4607174577787</v>
       </c>
-      <c r="K9" s="95"/>
-      <c r="L9" s="97"/>
-      <c r="M9" s="97" t="s">
+      <c r="K9" s="97"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="99" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O9" s="98" t="s">
+      <c r="O9" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P9" s="98"/>
+      <c r="P9" s="100"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -5862,7 +5866,7 @@
       <c r="U9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V9" s="17" t="n">
+      <c r="V9" s="24" t="n">
         <v>0.04714</v>
       </c>
       <c r="X9" s="3"/>
@@ -5879,44 +5883,44 @@
       <c r="AF9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="91" t="n">
+      <c r="A10" s="93" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="99" t="s">
+      <c r="D10" s="101" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="100" t="n">
+      <c r="F10" s="102" t="n">
         <v>22</v>
       </c>
-      <c r="G10" s="95"/>
-      <c r="H10" s="101"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="103"/>
       <c r="I10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="105" t="s">
+      <c r="J10" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="95"/>
-      <c r="L10" s="97"/>
-      <c r="M10" s="97" t="s">
+      <c r="K10" s="97"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="99" t="s">
         <v>40</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="98" t="s">
+      <c r="O10" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="98"/>
+      <c r="P10" s="100"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
@@ -5926,7 +5930,7 @@
       <c r="U10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="V10" s="17" t="n">
+      <c r="V10" s="24" t="n">
         <v>0.33</v>
       </c>
       <c r="X10" s="3"/>
@@ -5941,84 +5945,84 @@
       <c r="AF10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="67.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="106"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="108"/>
+      <c r="B11" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="107"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="110"/>
-      <c r="K11" s="108"/>
-      <c r="L11" s="111"/>
-      <c r="M11" s="111"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="112" t="s">
+      <c r="F11" s="109"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="110"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="113"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="112"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34" t="s">
+      <c r="P11" s="114"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="U11" s="29"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="113"/>
-      <c r="X11" s="34"/>
-      <c r="Y11" s="36" t="s">
+      <c r="U11" s="30"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="115"/>
+      <c r="X11" s="35"/>
+      <c r="Y11" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Z11" s="34"/>
-      <c r="AA11" s="34"/>
-      <c r="AB11" s="34"/>
-      <c r="AC11" s="38" t="s">
+      <c r="Z11" s="35"/>
+      <c r="AA11" s="35"/>
+      <c r="AB11" s="35"/>
+      <c r="AC11" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="AD11" s="37"/>
-      <c r="AE11" s="113"/>
-      <c r="AF11" s="39"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="115"/>
+      <c r="AF11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="114" t="n">
+      <c r="A12" s="116" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="42" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="94"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="94"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="97"/>
+      <c r="H12" s="96"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="96"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="93"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="95"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="98" t="s">
+      <c r="O12" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="98"/>
+      <c r="P12" s="100"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
@@ -6028,12 +6032,12 @@
       <c r="U12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V12" s="42" t="n">
+      <c r="V12" s="43" t="n">
         <f aca="false">SUM(V13:V21)</f>
         <v>0.34</v>
       </c>
       <c r="X12" s="3"/>
-      <c r="Y12" s="36" t="s">
+      <c r="Y12" s="37" t="s">
         <v>71</v>
       </c>
       <c r="Z12" s="3"/>
@@ -6048,44 +6052,44 @@
       <c r="AF12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="114" t="n">
+      <c r="A13" s="116" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="117" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="115" t="s">
+      <c r="D13" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="93" t="s">
+      <c r="E13" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="93" t="n">
+      <c r="F13" s="95" t="n">
         <v>7</v>
       </c>
-      <c r="G13" s="95"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="44" t="s">
+      <c r="G13" s="97"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="47" t="n">
+      <c r="J13" s="48" t="n">
         <v>54491472</v>
       </c>
-      <c r="K13" s="95"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="93" t="s">
+      <c r="K13" s="97"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="95" t="s">
         <v>40</v>
       </c>
       <c r="N13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O13" s="98" t="s">
+      <c r="O13" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="98"/>
+      <c r="P13" s="100"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11" t="n">
@@ -6097,7 +6101,7 @@
       <c r="U13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V13" s="46" t="n">
+      <c r="V13" s="47" t="n">
         <v>0.068</v>
       </c>
       <c r="X13" s="3"/>
@@ -6108,50 +6112,50 @@
         <v>3</v>
       </c>
       <c r="AC13" s="6"/>
-      <c r="AD13" s="41" t="s">
+      <c r="AD13" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="114" t="n">
+      <c r="A14" s="116" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C14" s="115" t="s">
+      <c r="C14" s="117" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="E14" s="93" t="s">
+      <c r="E14" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="93" t="n">
+      <c r="F14" s="95" t="n">
         <v>7</v>
       </c>
-      <c r="G14" s="95"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="44" t="s">
+      <c r="G14" s="97"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="K14" s="95"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="93" t="s">
+      <c r="K14" s="97"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="95" t="s">
         <v>40</v>
       </c>
       <c r="N14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O14" s="98" t="s">
+      <c r="O14" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="98"/>
+      <c r="P14" s="100"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11" t="n">
@@ -6163,7 +6167,7 @@
       <c r="U14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V14" s="46" t="n">
+      <c r="V14" s="47" t="n">
         <v>0.068</v>
       </c>
       <c r="X14" s="3"/>
@@ -6174,50 +6178,50 @@
         <v>3</v>
       </c>
       <c r="AC14" s="6"/>
-      <c r="AD14" s="41" t="s">
+      <c r="AD14" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="114" t="n">
+      <c r="A15" s="116" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C15" s="115" t="s">
+      <c r="C15" s="117" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="115" t="s">
+      <c r="D15" s="117" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="93" t="s">
+      <c r="E15" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="93" t="n">
+      <c r="F15" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="95"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="44" t="s">
+      <c r="G15" s="97"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="47" t="n">
+      <c r="J15" s="48" t="n">
         <v>5449000131836</v>
       </c>
-      <c r="K15" s="95"/>
-      <c r="L15" s="103"/>
-      <c r="M15" s="93" t="s">
+      <c r="K15" s="97"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="95" t="s">
         <v>40</v>
       </c>
       <c r="N15" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="98" t="s">
+      <c r="O15" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="98"/>
+      <c r="P15" s="100"/>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
       <c r="S15" s="11" t="n">
@@ -6229,7 +6233,7 @@
       <c r="U15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V15" s="46" t="n">
+      <c r="V15" s="47" t="n">
         <v>0.030226</v>
       </c>
       <c r="X15" s="3"/>
@@ -6240,50 +6244,50 @@
         <v>3</v>
       </c>
       <c r="AC15" s="6"/>
-      <c r="AD15" s="41" t="s">
+      <c r="AD15" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="114" t="n">
+      <c r="A16" s="116" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="115" t="s">
+      <c r="C16" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="115" t="s">
+      <c r="D16" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="93" t="s">
+      <c r="E16" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="93" t="n">
+      <c r="F16" s="95" t="n">
         <v>1</v>
       </c>
-      <c r="G16" s="95"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="44" t="s">
+      <c r="G16" s="97"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="47" t="n">
+      <c r="J16" s="48" t="n">
         <v>40822938</v>
       </c>
-      <c r="K16" s="95"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="93" t="s">
+      <c r="K16" s="97"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="95" t="s">
         <v>40</v>
       </c>
       <c r="N16" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="98" t="s">
+      <c r="O16" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="98"/>
+      <c r="P16" s="100"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
       <c r="S16" s="11" t="n">
@@ -6295,7 +6299,7 @@
       <c r="U16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V16" s="46" t="n">
+      <c r="V16" s="47" t="n">
         <v>0.015096</v>
       </c>
       <c r="X16" s="3"/>
@@ -6306,50 +6310,50 @@
         <v>3</v>
       </c>
       <c r="AC16" s="6"/>
-      <c r="AD16" s="41" t="s">
+      <c r="AD16" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="114" t="n">
+      <c r="A17" s="116" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C17" s="115" t="s">
+      <c r="C17" s="117" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="115" t="s">
+      <c r="D17" s="117" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="93" t="s">
+      <c r="E17" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="93" t="n">
+      <c r="F17" s="95" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="95"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="44" t="s">
+      <c r="G17" s="97"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="47" t="n">
+      <c r="J17" s="48" t="n">
         <v>54491069</v>
       </c>
-      <c r="K17" s="95"/>
-      <c r="L17" s="103"/>
-      <c r="M17" s="93" t="s">
+      <c r="K17" s="97"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="95" t="s">
         <v>40</v>
       </c>
       <c r="N17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O17" s="98" t="s">
+      <c r="O17" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="98"/>
+      <c r="P17" s="100"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11" t="n">
@@ -6361,7 +6365,7 @@
       <c r="U17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V17" s="46" t="n">
+      <c r="V17" s="47" t="n">
         <v>0.022678</v>
       </c>
       <c r="X17" s="3"/>
@@ -6372,50 +6376,50 @@
         <v>3</v>
       </c>
       <c r="AC17" s="6"/>
-      <c r="AD17" s="41" t="s">
+      <c r="AD17" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="114" t="n">
+      <c r="A18" s="116" t="n">
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="86" t="s">
+      <c r="C18" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="88" t="s">
         <v>161</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="93" t="n">
+      <c r="F18" s="95" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="95"/>
-      <c r="H18" s="93"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="95"/>
       <c r="I18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="J18" s="116" t="s">
+      <c r="J18" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="K18" s="95"/>
-      <c r="L18" s="103"/>
-      <c r="M18" s="93" t="s">
+      <c r="K18" s="97"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="95" t="s">
         <v>40</v>
       </c>
       <c r="N18" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O18" s="98" t="s">
+      <c r="O18" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P18" s="98"/>
+      <c r="P18" s="100"/>
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
       <c r="S18" s="11" t="n">
@@ -6427,7 +6431,7 @@
       <c r="U18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V18" s="46" t="n">
+      <c r="V18" s="47" t="n">
         <v>0.0226666666666667</v>
       </c>
       <c r="X18" s="3"/>
@@ -6438,50 +6442,50 @@
         <v>3</v>
       </c>
       <c r="AC18" s="6"/>
-      <c r="AD18" s="41" t="s">
+      <c r="AD18" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="114" t="n">
+      <c r="A19" s="116" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C19" s="86" t="s">
+      <c r="C19" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="88" t="s">
         <v>162</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="E19" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="93" t="n">
+      <c r="F19" s="95" t="n">
         <v>7</v>
       </c>
-      <c r="G19" s="95"/>
-      <c r="H19" s="93"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="95"/>
       <c r="I19" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="116" t="s">
+      <c r="J19" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="K19" s="95"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="93" t="s">
+      <c r="K19" s="97"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="95" t="s">
         <v>40</v>
       </c>
       <c r="N19" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O19" s="98" t="s">
+      <c r="O19" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P19" s="98"/>
+      <c r="P19" s="100"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11" t="n">
@@ -6493,7 +6497,7 @@
       <c r="U19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V19" s="46" t="n">
+      <c r="V19" s="47" t="n">
         <v>0.068</v>
       </c>
       <c r="X19" s="3"/>
@@ -6504,50 +6508,50 @@
         <v>3</v>
       </c>
       <c r="AC19" s="6"/>
-      <c r="AD19" s="41" t="s">
+      <c r="AD19" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="114" t="n">
+      <c r="A20" s="116" t="n">
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="115" t="s">
+      <c r="C20" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="115" t="s">
+      <c r="D20" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="93" t="s">
+      <c r="E20" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="93" t="n">
+      <c r="F20" s="95" t="n">
         <v>2</v>
       </c>
-      <c r="G20" s="95"/>
-      <c r="H20" s="93"/>
-      <c r="I20" s="44" t="s">
+      <c r="G20" s="97"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="47" t="n">
+      <c r="J20" s="48" t="n">
         <v>5449000189301</v>
       </c>
-      <c r="K20" s="95"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="97" t="s">
+      <c r="K20" s="97"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="99" t="s">
         <v>40</v>
       </c>
       <c r="N20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O20" s="98" t="s">
+      <c r="O20" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P20" s="98"/>
+      <c r="P20" s="100"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
       <c r="S20" s="11" t="n">
@@ -6559,7 +6563,7 @@
       <c r="U20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V20" s="46" t="n">
+      <c r="V20" s="47" t="n">
         <v>0.0226666666666667</v>
       </c>
       <c r="X20" s="3"/>
@@ -6570,50 +6574,50 @@
         <v>3</v>
       </c>
       <c r="AC20" s="6"/>
-      <c r="AD20" s="41" t="s">
+      <c r="AD20" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="114" t="n">
+      <c r="A21" s="116" t="n">
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="117" t="s">
+      <c r="D21" s="119" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="93" t="s">
+      <c r="E21" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="93" t="n">
+      <c r="F21" s="95" t="n">
         <v>2</v>
       </c>
-      <c r="G21" s="95"/>
-      <c r="H21" s="93"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="95"/>
       <c r="I21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="118" t="n">
+      <c r="J21" s="120" t="n">
         <v>4607174577787</v>
       </c>
-      <c r="K21" s="95"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="93" t="s">
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="95" t="s">
         <v>40</v>
       </c>
       <c r="N21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O21" s="98" t="s">
+      <c r="O21" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="P21" s="98"/>
+      <c r="P21" s="100"/>
       <c r="Q21" s="11"/>
       <c r="R21" s="3"/>
       <c r="S21" s="11" t="n">
@@ -6625,10 +6629,10 @@
       <c r="U21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="V21" s="46" t="n">
+      <c r="V21" s="47" t="n">
         <v>0.0226666666666667</v>
       </c>
-      <c r="X21" s="46"/>
+      <c r="X21" s="47"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
@@ -6636,15 +6640,15 @@
         <v>3</v>
       </c>
       <c r="AC21" s="6"/>
-      <c r="AD21" s="41" t="s">
+      <c r="AD21" s="42" t="s">
         <v>68</v>
       </c>
       <c r="AF21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K22" s="119"/>
-      <c r="L22" s="95"/>
-      <c r="M22" s="95"/>
+      <c r="K22" s="121"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AE21"/>
@@ -6676,43 +6680,43 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="121" t="s">
+      <c r="D1" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="121" t="s">
+      <c r="E1" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="121" t="s">
+      <c r="F1" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="121" t="s">
+      <c r="G1" s="123" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="121" t="s">
+      <c r="H1" s="123" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="121" t="s">
+      <c r="I1" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="121" t="s">
+      <c r="J1" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="121" t="s">
+      <c r="K1" s="123" t="s">
         <v>165</v>
       </c>
-      <c r="L1" s="121" t="s">
+      <c r="L1" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="121" t="s">
+      <c r="M1" s="123" t="s">
         <v>26</v>
       </c>
     </row>
@@ -6723,7 +6727,7 @@
       <c r="B3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="124" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>